<commit_message>
Use simplified keyboard model
The same keyboard description that is used for the virtual keyboard is
also used to translate physical keyboard scancodes.
</commit_message>
<xml_diff>
--- a/Keyboards.xlsx
+++ b/Keyboards.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="30" windowWidth="22995" windowHeight="10050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="us" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="292">
   <si>
     <t>Row</t>
   </si>
@@ -724,6 +724,174 @@
   </si>
   <si>
     <t>→</t>
+  </si>
+  <si>
+    <t>ScanCode</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>0B</t>
+  </si>
+  <si>
+    <t>0C</t>
+  </si>
+  <si>
+    <t>0D</t>
+  </si>
+  <si>
+    <t>0E</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>1F</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>E05B</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>E038</t>
+  </si>
+  <si>
+    <t>E05D</t>
+  </si>
+  <si>
+    <t>E01D</t>
   </si>
 </sst>
 </file>
@@ -767,7 +935,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -775,6 +962,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H86" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:H86"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="ScanCode" dataDxfId="0"/>
+    <tableColumn id="2" name="Row"/>
+    <tableColumn id="3" name="Column"/>
+    <tableColumn id="4" name="Width"/>
+    <tableColumn id="5" name="Label" dataDxfId="5"/>
+    <tableColumn id="6" name="Code" dataDxfId="4"/>
+    <tableColumn id="7" name="ShiftLabel" dataDxfId="3"/>
+    <tableColumn id="8" name="ShiftCode" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1064,1769 +1268,2034 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="7" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B6">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>12</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>14</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10">
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>16</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>18</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>20</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13">
         <v>0</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>22</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14">
         <v>0</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>24</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B15">
         <v>0</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>26</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B16">
         <v>0</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>28</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17">
         <v>0</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>30</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B18">
         <v>0</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>32</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>60</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20">
         <v>1</v>
       </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
       <c r="C20">
         <v>2</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>31</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21">
         <v>1</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>4</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1">
         <v>32</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>6</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1">
         <v>3</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>33</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23">
         <v>1</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>8</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
         <v>4</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>34</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>10</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1">
         <v>5</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>35</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25">
         <v>1</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>12</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="1">
         <v>6</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>36</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B26">
         <v>1</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>14</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1">
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1">
         <v>7</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>37</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B27">
         <v>1</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>16</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="1">
         <v>8</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>38</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B28">
         <v>1</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>18</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" s="1">
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
         <v>9</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>39</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B29">
         <v>1</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>20</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1">
         <v>0</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>30</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B30">
         <v>1</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>22</v>
       </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B31">
         <v>1</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>24</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B32">
         <v>1</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>26</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>6</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B33">
         <v>1</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>32</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>2</v>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
         <v>0</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>3</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2</v>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
         <v>3</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2</v>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>256</v>
       </c>
       <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
         <v>5</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>2</v>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>257</v>
       </c>
       <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
         <v>7</v>
       </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>2</v>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
         <v>9</v>
       </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="H38" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>2</v>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
         <v>11</v>
       </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>260</v>
       </c>
       <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
         <v>13</v>
       </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="H40" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2</v>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
         <v>15</v>
       </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>2</v>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>262</v>
       </c>
       <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
         <v>17</v>
       </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="H42" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>2</v>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
         <v>19</v>
       </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>2</v>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
         <v>21</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="H44" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2</v>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
         <v>23</v>
       </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G45" s="1" t="s">
+      <c r="H45" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>2</v>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
         <v>25</v>
       </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>2</v>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
         <v>27</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>5</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>2</v>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
         <v>32</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B49">
         <v>3</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>0</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>4</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B50">
         <v>3</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>4</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B51">
         <v>3</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>6</v>
       </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B52">
         <v>3</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>8</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B53">
         <v>3</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>10</v>
       </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="H53" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54">
         <v>3</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>12</v>
       </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54">
+        <v>2</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G54" s="1" t="s">
+      <c r="H54" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B55">
         <v>3</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>14</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56">
         <v>3</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>16</v>
       </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="F56" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="G56" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="H56" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B57">
         <v>3</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>18</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="G57" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="H57" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58">
         <v>3</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>20</v>
       </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="F58" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="H58" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59">
         <v>3</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>22</v>
       </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="F59" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="G59" s="1" t="s">
+      <c r="H59" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B60">
         <v>3</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>24</v>
       </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60" s="2" t="s">
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="F60" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B61">
         <v>3</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>26</v>
       </c>
-      <c r="C61">
+      <c r="D61">
+        <v>6</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <v>32</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B66">
+        <v>4</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67">
+        <v>4</v>
+      </c>
+      <c r="C67">
+        <v>11</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>17</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B71">
+        <v>4</v>
+      </c>
+      <c r="C71">
+        <v>19</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <v>21</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B73">
+        <v>4</v>
+      </c>
+      <c r="C73">
+        <v>23</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>25</v>
+      </c>
+      <c r="D74">
+        <v>7</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>32</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>4</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B77">
+        <v>5</v>
+      </c>
+      <c r="C77">
+        <v>4</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
         <v>8</v>
       </c>
-      <c r="D61" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62">
+      <c r="D79">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80">
+        <v>19</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>21</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82">
+        <v>23</v>
+      </c>
+      <c r="D82">
         <v>3</v>
       </c>
-      <c r="B62">
+      <c r="E82" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83">
+        <v>26</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>28</v>
+      </c>
+      <c r="D84">
+        <v>2</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="C85">
+        <v>30</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
         <v>32</v>
       </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>4</v>
-      </c>
-      <c r="B63">
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>5</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>5</v>
-      </c>
-      <c r="B64">
-        <v>5</v>
-      </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>5</v>
-      </c>
-      <c r="B65">
-        <v>7</v>
-      </c>
-      <c r="C65">
-        <v>2</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>9</v>
-      </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>5</v>
-      </c>
-      <c r="B67">
-        <v>11</v>
-      </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>5</v>
-      </c>
-      <c r="B68">
-        <v>13</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>5</v>
-      </c>
-      <c r="B69">
-        <v>15</v>
-      </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>5</v>
-      </c>
-      <c r="B70">
-        <v>17</v>
-      </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>5</v>
-      </c>
-      <c r="B71">
-        <v>19</v>
-      </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>5</v>
-      </c>
-      <c r="B72">
-        <v>21</v>
-      </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>5</v>
-      </c>
-      <c r="B73">
-        <v>23</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>5</v>
-      </c>
-      <c r="B74">
-        <v>25</v>
-      </c>
-      <c r="C74">
-        <v>7</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>5</v>
-      </c>
-      <c r="B75">
-        <v>32</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>6</v>
-      </c>
-      <c r="B76">
-        <v>0</v>
-      </c>
-      <c r="C76">
-        <v>4</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>6</v>
-      </c>
-      <c r="B77">
-        <v>4</v>
-      </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>6</v>
-      </c>
-      <c r="B78">
-        <v>6</v>
-      </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>6</v>
-      </c>
-      <c r="B79">
-        <v>8</v>
-      </c>
-      <c r="C79">
-        <v>11</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>6</v>
-      </c>
-      <c r="B80">
-        <v>19</v>
-      </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>6</v>
-      </c>
-      <c r="B81">
-        <v>21</v>
-      </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>6</v>
-      </c>
-      <c r="B82">
-        <v>23</v>
-      </c>
-      <c r="C82">
-        <v>3</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>6</v>
-      </c>
-      <c r="B83">
-        <v>26</v>
-      </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>6</v>
-      </c>
-      <c r="B84">
-        <v>28</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>6</v>
-      </c>
-      <c r="B85">
-        <v>30</v>
-      </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>6</v>
-      </c>
-      <c r="B86">
-        <v>32</v>
-      </c>
-      <c r="C86">
-        <v>2</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1" t="s">
         <v>231</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>